<commit_message>
fecha 3 russia 2018
</commit_message>
<xml_diff>
--- a/MatRumNam3614/resultados.xlsx
+++ b/MatRumNam3614/resultados.xlsx
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -437,11 +437,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="9" width="5.85546875" style="1" customWidth="1"/>
@@ -592,15 +592,15 @@
       </c>
       <c r="P3">
         <f>L5</f>
-        <v>0.58333333333333337</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="Q3">
         <f>L6</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="R3">
         <f>L7</f>
-        <v>0.33333333333333331</v>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -670,11 +670,11 @@
       </c>
       <c r="K5" s="1">
         <f>J5/SUM(J5:J7)</f>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="L5" s="1">
         <f>(J5+$M$1)/(SUM(J5:J7)+$M$1*3)</f>
-        <v>0.58333333333333337</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="N5" t="str">
         <f>A11</f>
@@ -701,17 +701,20 @@
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="1">
         <f>J6/SUM(J5:J7)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L6" s="1">
         <f>(J6+$M$1)/(SUM(J5:J7)+$M$1*3)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="N6" t="str">
         <f>A14</f>
@@ -747,11 +750,11 @@
       </c>
       <c r="K7" s="1">
         <f>J7/SUM(J5:J7)</f>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="L7" s="1">
         <f>(J7+$M$1)/(SUM(J5:J7)+$M$1*3)</f>
-        <v>0.33333333333333331</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="N7" t="str">
         <f>A17</f>
@@ -3753,15 +3756,15 @@
       </c>
       <c r="P71">
         <f>L209</f>
-        <v>0.72222222222222221</v>
+        <v>0.76190476190476186</v>
       </c>
       <c r="Q71">
         <f>L210</f>
-        <v>0.22222222222222221</v>
+        <v>0.19047619047619047</v>
       </c>
       <c r="R71">
         <f>L211</f>
-        <v>5.5555555555555552E-2</v>
+        <v>4.7619047619047616E-2</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
@@ -7816,6 +7819,9 @@
       <c r="C209" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D209" s="1">
+        <v>1</v>
+      </c>
       <c r="E209" s="1">
         <v>1</v>
       </c>
@@ -7830,15 +7836,15 @@
       </c>
       <c r="J209" s="4">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K209" s="1">
         <f>J209/SUM(J209:J211)</f>
-        <v>0.8</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="L209" s="1">
         <f>(J209+$M$1)/(SUM(J209:J211)+$M$1*3)</f>
-        <v>0.72222222222222221</v>
+        <v>0.76190476190476186</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -7854,11 +7860,11 @@
       </c>
       <c r="K210" s="1">
         <f>J210/SUM(J209:J211)</f>
-        <v>0.2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="L210" s="1">
         <f>(J210+$M$1)/(SUM(J209:J211)+$M$1*3)</f>
-        <v>0.22222222222222221</v>
+        <v>0.19047619047619047</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.2">
@@ -7875,7 +7881,7 @@
       </c>
       <c r="L211" s="1">
         <f>(J211+$M$1)/(SUM(J209:J211)+$M$1*3)</f>
-        <v>5.5555555555555552E-2</v>
+        <v>4.7619047619047616E-2</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>